<commit_message>
prefab-v0.0.1, renamed world, updated rendering
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27660" windowHeight="11140" activeTab="4"/>
+    <workbookView windowWidth="27660" windowHeight="11140" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="mob" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="drop" sheetId="3" r:id="rId3"/>
     <sheet name="rarity" sheetId="4" r:id="rId4"/>
     <sheet name="level" sheetId="5" r:id="rId5"/>
-    <sheet name="legacy" sheetId="6" r:id="rId6"/>
+    <sheet name="tag" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -1812,7 +1812,7 @@
   </sheetPr>
   <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="J94" sqref="J94"/>
@@ -4065,7 +4065,7 @@
         <v>100</v>
       </c>
       <c r="B102" s="3">
-        <f>ROUND(B101*1.095,-5)</f>
+        <f t="shared" si="13"/>
         <v>2600000</v>
       </c>
       <c r="C102" s="3">
@@ -4118,7 +4118,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>

</xml_diff>

<commit_message>
prefab-v0.0.2, optimized rendering, perm system
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27660" windowHeight="11140"/>
+    <workbookView windowWidth="27660" windowHeight="11140" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="mob" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="51">
   <si>
     <t>health</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>slot</t>
+  </si>
+  <si>
+    <t>{"sight": 5}</t>
   </si>
 </sst>
 </file>
@@ -1176,7 +1179,7 @@
   </sheetPr>
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
@@ -1858,10 +1861,10 @@
   </sheetPr>
   <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="J94" sqref="J94"/>
+      <selection pane="bottomLeft" activeCell="F103" sqref="F103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -4147,7 +4150,7 @@
         <v>1000</v>
       </c>
       <c r="F103" s="5" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prefab-v0.0.2, changed mob, perm check
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27660" windowHeight="11140" activeTab="4"/>
+    <workbookView windowWidth="27660" windowHeight="11140"/>
   </bookViews>
   <sheets>
     <sheet name="mob" sheetId="1" r:id="rId1"/>
@@ -1179,10 +1179,10 @@
   </sheetPr>
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="2"/>
@@ -1237,7 +1237,7 @@
         <v>0.2</v>
       </c>
       <c r="D2" s="10">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
@@ -1269,7 +1269,7 @@
         <v>0.2</v>
       </c>
       <c r="D3" s="11">
-        <v>0.01</v>
+        <v>0.6</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -1861,8 +1861,8 @@
   </sheetPr>
   <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="F103" sqref="F103"/>
     </sheetView>

</xml_diff>

<commit_message>
prefab-0.0.4, fake wall, system, rendering
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="73">
   <si>
     <t>health</t>
   </si>
@@ -171,7 +171,70 @@
     <t>slot</t>
   </si>
   <si>
-    <t>{"sight":1.5}</t>
+    <t>{"sight":1.5,"speed":22.0}</t>
+  </si>
+  <si>
+    <t>{"sight":1.5,"speed":22.1}</t>
+  </si>
+  <si>
+    <t>{"sight":1.5,"speed":22.2}</t>
+  </si>
+  <si>
+    <t>{"sight":1.5,"speed":22.3}</t>
+  </si>
+  <si>
+    <t>{"sight":1.5,"speed":22.4}</t>
+  </si>
+  <si>
+    <t>{"sight":1.5,"speed":22.5}</t>
+  </si>
+  <si>
+    <t>{"sight":1.5,"speed":22.6}</t>
+  </si>
+  <si>
+    <t>{"sight":1.5,"speed":22.7}</t>
+  </si>
+  <si>
+    <t>{"sight":1.5,"speed":22.8}</t>
+  </si>
+  <si>
+    <t>{"sight":1.5,"speed":22.9}</t>
+  </si>
+  <si>
+    <t>{"sight":1.5,"speed":23.0}</t>
+  </si>
+  <si>
+    <t>{"sight":1.5,"speed":23.1}</t>
+  </si>
+  <si>
+    <t>{"sight":1.5,"speed":23.2}</t>
+  </si>
+  <si>
+    <t>{"sight":1.5,"speed":23.3}</t>
+  </si>
+  <si>
+    <t>{"sight":1.5,"speed":23.4}</t>
+  </si>
+  <si>
+    <t>{"sight":1.5,"speed":23.5}</t>
+  </si>
+  <si>
+    <t>{"sight":1.5,"speed":23.6}</t>
+  </si>
+  <si>
+    <t>{"sight":1.5,"speed":23.7}</t>
+  </si>
+  <si>
+    <t>{"sight":1.5,"speed":23.8}</t>
+  </si>
+  <si>
+    <t>{"sight":1.5,"speed":23.9}</t>
+  </si>
+  <si>
+    <t>{"sight":1.5,"speed":24}</t>
+  </si>
+  <si>
+    <t>{"sight": 2.5, "speed":25}</t>
   </si>
   <si>
     <t>{"sight": 2.5}</t>
@@ -1867,7 +1930,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="5"/>
@@ -1876,7 +1939,7 @@
     <col min="2" max="2" width="9.625" style="1" customWidth="1"/>
     <col min="3" max="4" width="12.375" style="1" customWidth="1"/>
     <col min="5" max="5" width="12.25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="21.375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1" spans="2:6">
@@ -1933,7 +1996,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" ht="17.25" customHeight="1" spans="1:6">
@@ -1953,7 +2016,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" ht="17.25" customHeight="1" spans="1:6">
@@ -1973,7 +2036,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" ht="17.25" customHeight="1" spans="1:6">
@@ -1994,7 +2057,7 @@
         <v>10</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" ht="17.25" customHeight="1" spans="1:6">
@@ -2014,7 +2077,7 @@
         <v>11</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" ht="17.25" customHeight="1" spans="1:6">
@@ -2034,7 +2097,7 @@
         <v>11</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" ht="17.25" customHeight="1" spans="1:6">
@@ -2054,7 +2117,7 @@
         <v>12</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" ht="17.25" customHeight="1" spans="1:6">
@@ -2074,7 +2137,7 @@
         <v>12</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" ht="17.25" customHeight="1" spans="1:6">
@@ -2094,7 +2157,7 @@
         <v>13</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" ht="17.25" customHeight="1" spans="1:6">
@@ -2114,7 +2177,7 @@
         <v>13</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" ht="17.25" customHeight="1" spans="1:6">
@@ -2134,7 +2197,7 @@
         <v>14</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" ht="17.25" customHeight="1" spans="1:6">
@@ -2154,7 +2217,7 @@
         <v>14</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" ht="17.25" customHeight="1" spans="1:6">
@@ -2174,7 +2237,7 @@
         <v>15</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" ht="17.25" customHeight="1" spans="1:6">
@@ -2194,7 +2257,7 @@
         <v>15</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" ht="17.25" customHeight="1" spans="1:6">
@@ -2214,7 +2277,7 @@
         <v>16</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" ht="17.25" customHeight="1" spans="1:6">
@@ -2234,7 +2297,7 @@
         <v>16</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" ht="17.25" customHeight="1" spans="1:6">
@@ -2254,7 +2317,7 @@
         <v>17</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" ht="17.25" customHeight="1" spans="1:6">
@@ -2274,7 +2337,7 @@
         <v>18</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" ht="17.25" customHeight="1" spans="1:6">
@@ -2294,7 +2357,7 @@
         <v>19</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" ht="17.25" customHeight="1" spans="1:6">
@@ -2314,7 +2377,7 @@
         <v>20</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" ht="17.25" customHeight="1" spans="1:6">
@@ -4153,7 +4216,7 @@
         <v>1000</v>
       </c>
       <c r="F103" s="5" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -4174,7 +4237,7 @@
         <v>1000</v>
       </c>
       <c r="F104" s="4" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>